<commit_message>
Customer Migration changes and customer aproval
</commit_message>
<xml_diff>
--- a/customerOnboarding.xlsx
+++ b/customerOnboarding.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E8422C-32BA-40CA-8757-F11E879C664B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC6B167-1616-4F06-A5DA-1F49999B7667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="122">
   <si>
     <t>Account Title</t>
   </si>
@@ -358,6 +358,36 @@
   </si>
   <si>
     <t>GERMANY</t>
+  </si>
+  <si>
+    <t>Identity Type</t>
+  </si>
+  <si>
+    <t>ARC</t>
+  </si>
+  <si>
+    <t>NICOP</t>
+  </si>
+  <si>
+    <t>L0 BVS User</t>
+  </si>
+  <si>
+    <t>Permanent Province</t>
+  </si>
+  <si>
+    <t>Gilgit Baltistan</t>
+  </si>
+  <si>
+    <t>KPK</t>
+  </si>
+  <si>
+    <t>Mailing Province</t>
+  </si>
+  <si>
+    <t>Azad Jammu Kashmir</t>
+  </si>
+  <si>
+    <t>Sindh</t>
   </si>
 </sst>
 </file>
@@ -710,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K3" sqref="K1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,17 +754,19 @@
     <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,25 +792,34 @@
         <v>108</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -804,25 +845,34 @@
         <v>109</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -848,22 +898,31 @@
         <v>110</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>19</v>
+      <c r="Q3" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -874,10 +933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D730AAB-C629-46C5-9B47-EC7DBE6D6233}">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,12 +945,15 @@
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="28" width="9.140625" style="1"/>
-    <col min="29" max="29" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="29" width="9.140625" style="1"/>
+    <col min="30" max="30" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -914,73 +976,82 @@
         <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1006,70 +1077,79 @@
         <v>109</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -1095,66 +1175,75 @@
         <v>111</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1166,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB3A3B2-CAB1-4060-9240-1826448BDB42}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,14 +1266,17 @@
     <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="29" width="9.140625" style="1"/>
-    <col min="30" max="30" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="30" width="9.140625" style="1"/>
+    <col min="31" max="31" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -1203,80 +1295,83 @@
       <c r="F1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -1296,79 +1391,82 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>82</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -1388,82 +1486,85 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>82</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{B5674DA0-F58B-4F04-B73B-DD31353A776E}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{E6FF78C6-E195-4F2A-9CF8-2DBC75C69467}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{B5674DA0-F58B-4F04-B73B-DD31353A776E}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{E6FF78C6-E195-4F2A-9CF8-2DBC75C69467}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>